<commit_message>
teste conversao de texto pra numero
</commit_message>
<xml_diff>
--- a/produtos.xlsx
+++ b/produtos.xlsx
@@ -432,7 +432,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -460,68 +460,68 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>seleção biscoitos de natal 300g</t>
+          <t>cookies limão 140g</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$44.90</t>
+          <t>R$20.99</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$39.90</t>
+          <t>R$19.99</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>cookies com gotas ao leite 120g</t>
+          <t>cookies 3 chocolates 140g</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$17.90</t>
+          <t>R$20.99</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$16.90</t>
+          <t>R$19.99</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>cookies duo chocolate 120g</t>
+          <t>cookies com gotas ao leite 120g</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$17.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>R$16.90</t>
+          <t>R$16.99</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>cookies natal gotas ao leite 140g</t>
+          <t>wafer mil folhas 80g</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$17.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$16.90</t>
+          <t>R$15.99</t>
         </is>
       </c>
     </row>
@@ -533,29 +533,29 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$16.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$14.90</t>
+          <t>R$15.99</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>wafer mil folhas 80g</t>
+          <t>wafer cappuccino 80g</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$16.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$14.90</t>
+          <t>R$15.99</t>
         </is>
       </c>
     </row>
@@ -567,114 +567,199 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$16.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$14.90</t>
+          <t>R$15.99</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>biscoito tradicional ao leite 100g</t>
+          <t>cookies duo chocolate 120g</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$16.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$14.90</t>
+          <t>R$16.99</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>biscoito tradicional coberto ao leite 50g</t>
+          <t>biscoito tradicional ao leite 100g</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$9.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$8.90</t>
+          <t>R$15.99</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>biscoito caramelizado 100g</t>
+          <t>wafer limão 80g</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$9.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$8.90</t>
+          <t>R$15.99</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>pão de mel doce de leite 50g</t>
+          <t>wafer coberto ao leite 80g</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R$8.90</t>
+          <t>R$17.99</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$8.50</t>
+          <t>R$16.99</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>bytes wafer avelã 50g</t>
+          <t>pão de mel doce de leite 50g</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R$9.50</t>
+          <t>R$11.99</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$8.90</t>
+          <t>R$9.99</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>biscoito tradicional coberto ao leite 50g</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R$10.99</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>R$9.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>cookies tradicional gotas ao leite 40g</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>R$10.99</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>R$9.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>biscoito caramelizado 100g</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>R$10.99</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>R$9.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>biscoito caramelizado coberto ao leite 50g</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>R$10.99</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>R$9.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>bytes wafer avelã 50g</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>R$10.59</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>R$9.99</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>wafer bytes sintonia 45g</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R$8.50</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>R$7.90</t>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>R$10.59</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>R$9.99</t>
         </is>
       </c>
     </row>

</xml_diff>